<commit_message>
update auto test Register
</commit_message>
<xml_diff>
--- a/test-resources/data/TEST_CHANGEPASSWORD.xlsx
+++ b/test-resources/data/TEST_CHANGEPASSWORD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoct\Desktop\KiemThuNangCao\ASM\Poly.Asg\test-resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA2\GodEshop\test-resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BEB612-87B9-4BE8-AD80-6BB23B8CD769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DADB70-4458-400C-B4F0-82CACF8BAE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31A90451-6911-4571-A036-C38FC9F55ECC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31A90451-6911-4571-A036-C38FC9F55ECC}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -52,20 +52,44 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>user02</t>
-  </si>
-  <si>
     <t>SUCCESS</t>
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>cust01</t>
+  </si>
+  <si>
+    <t>nghiattps14820@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>Matkhau@123</t>
+  </si>
+  <si>
+    <t>Matkhau@1234</t>
+  </si>
+  <si>
+    <t>Matkhau@124</t>
+  </si>
+  <si>
+    <t>Matkhau@1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,16 +97,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,14 +141,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,136 +489,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69647681-E2BC-4E80-81BF-D5D25DAD6159}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="16.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>123</v>
-      </c>
-      <c r="D2">
-        <v>12345</v>
-      </c>
-      <c r="E2">
-        <v>12345</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>12345</v>
-      </c>
-      <c r="E3">
-        <v>12345</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>123456</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>123456</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>123</v>
-      </c>
-      <c r="D4">
-        <v>12345</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>123</v>
-      </c>
-      <c r="E5">
-        <v>12345</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>123</v>
-      </c>
-      <c r="D6">
-        <v>12345</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1EA1E6CE-0D63-42BD-9DBD-D9C2E48C64E2}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{81B3BB74-CA14-481D-A67D-2030BB63483C}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{7CB78D65-C702-4A93-833E-C75B34848BFA}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{04D6E4C7-B453-4109-89F7-2C6B7643BA5C}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{85AA1490-910C-499E-9D10-B21A4554DAEE}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{5F443879-D0C9-4F92-A4CB-FEA1E23F9907}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{A593B882-EBD3-4735-BA29-C771F7E60ECA}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{1C00317B-C9B9-4EEC-93AB-ED36FF3D520B}"/>
+    <hyperlink ref="G4" r:id="rId9" xr:uid="{FE36AD3D-8382-40E3-BDBF-069BE50E58F1}"/>
+    <hyperlink ref="E5" r:id="rId10" xr:uid="{CD2B8E13-D644-4085-BC3C-58F899C3D491}"/>
+    <hyperlink ref="G5" r:id="rId11" xr:uid="{CE47757F-74A4-4AEC-9B43-FB850E0AE8D7}"/>
+    <hyperlink ref="E6" r:id="rId12" xr:uid="{2A957CCD-1365-4743-90B5-3280A1964A6F}"/>
+    <hyperlink ref="F6" r:id="rId13" xr:uid="{AC56A67B-BCFB-489F-B603-4B8085C945B7}"/>
+    <hyperlink ref="F7" r:id="rId14" xr:uid="{4A79C17C-54AE-42D5-BB48-FC893DA22992}"/>
+    <hyperlink ref="G7" r:id="rId15" xr:uid="{88AFA10B-9E8F-4465-8C12-6D9673D71E24}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>